<commit_message>
Adds anotated 05 video + new results
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14680" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>game_00</t>
   </si>
@@ -44,10 +44,10 @@
     <t>game_04</t>
   </si>
   <si>
-    <t>detekovaných události</t>
+    <t>chybějící doteky</t>
   </si>
   <si>
-    <t>anotované události</t>
+    <t>chybějící góly</t>
   </si>
   <si>
     <t xml:space="preserve">doteky chybějící </t>
@@ -61,15 +61,78 @@
   <si>
     <t xml:space="preserve">góly navíc </t>
   </si>
+  <si>
+    <t xml:space="preserve">události anotované </t>
+  </si>
+  <si>
+    <t>události detekované</t>
+  </si>
+  <si>
+    <t>doteky správně</t>
+  </si>
+  <si>
+    <t>góly správně</t>
+  </si>
+  <si>
+    <t>anotované</t>
+  </si>
+  <si>
+    <t>doteky anotované</t>
+  </si>
+  <si>
+    <t>góly anotované</t>
+  </si>
+  <si>
+    <t>detekované správně</t>
+  </si>
+  <si>
+    <t>doteky navíc</t>
+  </si>
+  <si>
+    <t>góly navíc</t>
+  </si>
+  <si>
+    <t>Vyhodnocení gólů</t>
+  </si>
+  <si>
+    <t>Vyhodnocení doteků</t>
+  </si>
+  <si>
+    <t>game_05</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,7 +146,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -91,15 +154,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hypertextový odkaz" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Použitý hypertextový odkaz" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Použitý hypertextový odkaz" xfId="4" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -112,6 +201,315 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="cs-CZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1"/>
+              <a:t>Vyhodnocení doteků</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>List1!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vyhodnocení doteků</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>List1!$A$20:$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>anotované</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>detekované správně</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>chybějící doteky</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>doteky navíc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>List1!$B$20:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>390.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>263.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>127.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>116.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1869359696"/>
+        <c:axId val="1867840080"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1869359696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1867840080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1867840080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="320.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1869359696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="40.0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="cs-CZ"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="cs-CZ"/>
@@ -140,7 +538,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -168,11 +566,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>List1!$B$1</c:f>
+              <c:f>List1!$B$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>game_00</c:v>
+                  <c:v>Vyhodnocení gólů</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -189,365 +587,41 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>List1!$A$2:$A$7</c:f>
+              <c:f>List1!$A$27:$A$30</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>anotované události</c:v>
+                  <c:v>anotované</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>detekovaných události</c:v>
+                  <c:v>detekované správně</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>doteky chybějící </c:v>
+                  <c:v>chybějící góly</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>doteky navíc </c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>góly chybějící </c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>góly navíc </c:v>
+                  <c:v>góly navíc</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>List1!$B$2:$B$7</c:f>
+              <c:f>List1!$B$27:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>48.0</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>List1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>game_01</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>List1!$A$2:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>anotované události</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>detekovaných události</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>doteky chybějící </c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>doteky navíc </c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>góly chybějící </c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>góly navíc </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>List1!$C$2:$C$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>92.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>81.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>33.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>List1!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>game_02</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>List1!$A$2:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>anotované události</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>detekovaných události</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>doteky chybějící </c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>doteky navíc </c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>góly chybějící </c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>góly navíc </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>List1!$D$2:$D$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>66.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>65.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>List1!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>game_03</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>List1!$A$2:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>anotované události</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>detekovaných události</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>doteky chybějící </c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>doteky navíc </c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>góly chybějící </c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>góly navíc </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>List1!$E$2:$E$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>70.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>87.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>34.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>List1!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>game_04</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>List1!$A$2:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>anotované události</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>detekovaných události</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>doteky chybějící </c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>doteky navíc </c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>góly chybějící </c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>góly navíc </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>List1!$F$2:$F$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>66.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>54.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>23.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -563,11 +637,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1867733344"/>
-        <c:axId val="1796961392"/>
+        <c:axId val="1759201024"/>
+        <c:axId val="1898743840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1867733344"/>
+        <c:axId val="1759201024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -595,7 +669,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -610,7 +684,7 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1796961392"/>
+        <c:crossAx val="1898743840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -618,9 +692,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1796961392"/>
+        <c:axId val="1898743840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="22.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -638,7 +713,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -654,7 +728,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -669,9 +743,10 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1867733344"/>
+        <c:crossAx val="1759201024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="2.0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -681,38 +756,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="cs-CZ"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -790,6 +833,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1293,24 +1376,527 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Graf 6"/>
+        <xdr:cNvPr id="23" name="Graf 22"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1320,6 +1906,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="24" name="Graf 23"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1591,18 +2207,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1618,10 +2236,13 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>48</v>
@@ -1638,105 +2259,305 @@
       <c r="F2">
         <v>66</v>
       </c>
+      <c r="G2">
+        <v>76</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4">
+        <v>49</v>
+      </c>
+      <c r="C3" s="4">
+        <v>81</v>
+      </c>
+      <c r="D3" s="4">
+        <v>65</v>
+      </c>
+      <c r="E3" s="4">
+        <v>87</v>
+      </c>
+      <c r="F3" s="4">
+        <v>54</v>
+      </c>
+      <c r="G3" s="5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>44</v>
+      </c>
+      <c r="C4">
+        <v>86</v>
+      </c>
+      <c r="D4">
+        <v>62</v>
+      </c>
+      <c r="E4">
+        <v>65</v>
+      </c>
+      <c r="F4">
+        <v>63</v>
+      </c>
+      <c r="G4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>37</v>
+      </c>
+      <c r="C5">
+        <v>53</v>
+      </c>
+      <c r="D5">
+        <v>45</v>
+      </c>
+      <c r="E5">
+        <v>47</v>
+      </c>
+      <c r="F5">
+        <v>40</v>
+      </c>
+      <c r="G5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>33</v>
+      </c>
+      <c r="D6">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>23</v>
+      </c>
+      <c r="G6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>22</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>34</v>
+      </c>
+      <c r="F7">
+        <v>12</v>
+      </c>
+      <c r="G7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>49</v>
-      </c>
-      <c r="C3">
-        <v>81</v>
-      </c>
-      <c r="D3">
-        <v>65</v>
-      </c>
-      <c r="E3">
-        <v>87</v>
-      </c>
-      <c r="F3">
-        <v>54</v>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>33</v>
-      </c>
-      <c r="D4">
-        <v>17</v>
-      </c>
-      <c r="E4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <f>SUM($B4:$G4)</f>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="F4">
-        <v>23</v>
+      <c r="B21">
+        <f t="shared" ref="B21:B24" si="0">SUM($B5:$G5)</f>
+        <v>263</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>22</v>
-      </c>
-      <c r="D5">
-        <v>16</v>
-      </c>
-      <c r="E5">
-        <v>34</v>
-      </c>
-      <c r="F5">
-        <v>12</v>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <f>SUM($B9:$G9)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28">
+        <f t="shared" ref="B28:B30" si="1">SUM($B10:$G10)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>